<commit_message>
Added python diagrams for Leake amphiboles
</commit_message>
<xml_diff>
--- a/Benchmarking/amphibole/Python_Amphiboles_Test.xlsx
+++ b/Benchmarking/amphibole/Python_Amphiboles_Test.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/wieserp_oregonstate_edu/Documents/Postdoc/PyMME/MyBarometers/Thermobar_outer/Benchmarking/amphibole/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Benchmarking\amphibole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3A5CF295-058B-4B8E-AB28-A6DCAB2B1D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C116E292-B288-4B9B-8D10-222D70D49E48}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4792ACAF-1EE3-4CE0-A8D6-4D57D458A076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{2178F5D2-4A6B-4AB8-B064-27A64C9B3448}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{2178F5D2-4A6B-4AB8-B064-27A64C9B3448}"/>
   </bookViews>
   <sheets>
     <sheet name="Putirka_Benchmarks" sheetId="1" r:id="rId1"/>
-    <sheet name="Ridolfi2012" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Ridolfi2012" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1011,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30858796-A7D8-4C33-BDED-A78CC9678424}">
   <dimension ref="A1:BA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4757,6 +4758,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC75D0C1-29C5-44F4-85E9-AC6CBA4BA398}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409558E-BB15-4A45-8836-B2357CF4DB7C}">
   <dimension ref="A1:T73"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added element to oxide, Keith Si equation, Before messed with labelling
</commit_message>
<xml_diff>
--- a/Benchmarking/amphibole/Python_Amphiboles_Test.xlsx
+++ b/Benchmarking/amphibole/Python_Amphiboles_Test.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Benchmarking\amphibole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4792ACAF-1EE3-4CE0-A8D6-4D57D458A076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB40C30B-180A-4689-9A50-BB8492ABE499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{2178F5D2-4A6B-4AB8-B064-27A64C9B3448}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{2178F5D2-4A6B-4AB8-B064-27A64C9B3448}"/>
   </bookViews>
   <sheets>
-    <sheet name="Putirka_Benchmarks" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Ridolfi2012" sheetId="2" r:id="rId3"/>
+    <sheet name="Info" sheetId="4" r:id="rId1"/>
+    <sheet name="Putirka_Benchmarks" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Ridolfi2012" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -400,6 +401,15 @@
   </si>
   <si>
     <t>P_Choice</t>
+  </si>
+  <si>
+    <t>Putirka_Benchmarks reads from Putirka_Amphibole P-T_v.6_downMay2021.xlsx, the most up-to-date version</t>
+  </si>
+  <si>
+    <t>SiO2_Calc</t>
+  </si>
+  <si>
+    <t>T_C_SiO2_Calc</t>
   </si>
 </sst>
 </file>
@@ -1009,11 +1019,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A54A30-9156-49FD-9617-C3373B239D83}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30858796-A7D8-4C33-BDED-A78CC9678424}">
-  <dimension ref="A1:BA23"/>
+  <dimension ref="A1:BC23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1052,7 @@
     <col min="27" max="27" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="10" customFormat="1" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" s="10" customFormat="1" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1182,8 +1212,14 @@
       <c r="BA1" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC1" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1344,8 +1380,14 @@
         <f>AZ2+273.15</f>
         <v>1226.8469601940619</v>
       </c>
-    </row>
-    <row r="3" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB2">
+        <v>57.936794676762176</v>
+      </c>
+      <c r="BC2">
+        <v>955.93956668022042</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1507,8 +1549,14 @@
         <f t="shared" ref="BA3:BA23" si="0">AZ3+273.15</f>
         <v>1192.4328347296389</v>
       </c>
-    </row>
-    <row r="4" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB3">
+        <v>63.369069414151781</v>
+      </c>
+      <c r="BC3">
+        <v>911.89573022935838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1670,8 +1718,14 @@
         <f t="shared" si="0"/>
         <v>1241.3464919380276</v>
       </c>
-    </row>
-    <row r="5" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB4">
+        <v>55.154572604355693</v>
+      </c>
+      <c r="BC4">
+        <v>978.97328086757784</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1833,8 +1887,14 @@
         <f t="shared" si="0"/>
         <v>1217.1567830709282</v>
       </c>
-    </row>
-    <row r="6" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB5">
+        <v>62.682265934371905</v>
+      </c>
+      <c r="BC5">
+        <v>935.43054369867843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1996,8 +2056,14 @@
         <f t="shared" si="0"/>
         <v>1202.5197116318166</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB6">
+        <v>64.774797714210138</v>
+      </c>
+      <c r="BC6">
+        <v>914.6345629403919</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2159,8 +2225,14 @@
         <f t="shared" si="0"/>
         <v>1230.6516188253704</v>
       </c>
-    </row>
-    <row r="8" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB7">
+        <v>60.056929592101881</v>
+      </c>
+      <c r="BC7">
+        <v>958.5507702281169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2322,8 +2394,14 @@
         <f t="shared" si="0"/>
         <v>1212.9742296567108</v>
       </c>
-    </row>
-    <row r="9" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB8">
+        <v>62.538583166103997</v>
+      </c>
+      <c r="BC8">
+        <v>932.88405708448386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2485,8 +2563,14 @@
         <f t="shared" si="0"/>
         <v>1193.6349096032995</v>
       </c>
-    </row>
-    <row r="10" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB9">
+        <v>64.0207866165794</v>
+      </c>
+      <c r="BC9">
+        <v>908.93954404667261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2648,8 +2732,14 @@
         <f t="shared" si="0"/>
         <v>1226.7145644875991</v>
       </c>
-    </row>
-    <row r="11" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB10">
+        <v>60.044381225346953</v>
+      </c>
+      <c r="BC10">
+        <v>954.78564773000312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2811,8 +2901,14 @@
         <f t="shared" si="0"/>
         <v>1242.5489436747853</v>
       </c>
-    </row>
-    <row r="12" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB11">
+        <v>53.105290465119687</v>
+      </c>
+      <c r="BC11">
+        <v>975.82496756237549</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2974,8 +3070,14 @@
         <f t="shared" si="0"/>
         <v>1233.6773864662991</v>
       </c>
-    </row>
-    <row r="13" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB12">
+        <v>54.037494320022375</v>
+      </c>
+      <c r="BC12">
+        <v>964.69486450788281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3137,8 +3239,14 @@
         <f t="shared" si="0"/>
         <v>1249.0697545386852</v>
       </c>
-    </row>
-    <row r="14" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB13">
+        <v>52.079901953608392</v>
+      </c>
+      <c r="BC13">
+        <v>985.92565312692466</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3299,8 +3407,14 @@
         <f t="shared" si="0"/>
         <v>1224.8523425333442</v>
       </c>
-    </row>
-    <row r="15" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB14">
+        <v>57.936794676762176</v>
+      </c>
+      <c r="BC14">
+        <v>955.93956668022042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3461,8 +3575,14 @@
         <f t="shared" si="0"/>
         <v>1191.0684104313486</v>
       </c>
-    </row>
-    <row r="16" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB15">
+        <v>63.369069414151781</v>
+      </c>
+      <c r="BC15">
+        <v>911.89573022935838</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3623,8 +3743,14 @@
         <f t="shared" si="0"/>
         <v>1240.382273508852</v>
       </c>
-    </row>
-    <row r="17" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB16">
+        <v>55.154572604355693</v>
+      </c>
+      <c r="BC16">
+        <v>978.97328086757784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3783,8 +3909,14 @@
         <f t="shared" si="0"/>
         <v>1092.0246971411957</v>
       </c>
-    </row>
-    <row r="18" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="BB17">
+        <v>72.270201280929896</v>
+      </c>
+      <c r="BC17">
+        <v>807.47189104003451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3943,8 +4075,14 @@
         <f t="shared" si="0"/>
         <v>1087.464264545376</v>
       </c>
-    </row>
-    <row r="19" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB18">
+        <v>73.502618363842714</v>
+      </c>
+      <c r="BC18">
+        <v>793.17204982520741</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4103,8 +4241,14 @@
         <f t="shared" si="0"/>
         <v>1087.464264545376</v>
       </c>
-    </row>
-    <row r="20" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB19">
+        <v>73.502618363842714</v>
+      </c>
+      <c r="BC19">
+        <v>793.17204982520741</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4265,8 +4409,14 @@
         <f t="shared" si="0"/>
         <v>1026.5583759929586</v>
       </c>
-    </row>
-    <row r="21" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB20">
+        <v>65.139424765079326</v>
+      </c>
+      <c r="BC20">
+        <v>684.6109011016058</v>
+      </c>
+    </row>
+    <row r="21" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4427,8 +4577,14 @@
         <f t="shared" si="0"/>
         <v>1029.5814034495259</v>
       </c>
-    </row>
-    <row r="22" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB21">
+        <v>65.525355917219827</v>
+      </c>
+      <c r="BC21">
+        <v>690.99385346086331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4589,8 +4745,14 @@
         <f t="shared" si="0"/>
         <v>1137.2065563759165</v>
       </c>
-    </row>
-    <row r="23" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB22">
+        <v>68.398915624742628</v>
+      </c>
+      <c r="BC22">
+        <v>791.56115992271941</v>
+      </c>
+    </row>
+    <row r="23" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4750,6 +4912,12 @@
       <c r="BA23">
         <f t="shared" si="0"/>
         <v>1113.0170396903568</v>
+      </c>
+      <c r="BB23">
+        <v>63.258429461137496</v>
+      </c>
+      <c r="BC23">
+        <v>809.75166252155498</v>
       </c>
     </row>
   </sheetData>
@@ -4757,11 +4925,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC75D0C1-29C5-44F4-85E9-AC6CBA4BA398}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -4863,7 +5031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409558E-BB15-4A45-8836-B2357CF4DB7C}">
   <dimension ref="A1:T73"/>
   <sheetViews>

</xml_diff>